<commit_message>
heatmap for cc-pvdz added
</commit_message>
<xml_diff>
--- a/hexabenzocoronene/sto3g/est_basis/hexabenzocorornene_faraday_discussion.xlsx
+++ b/hexabenzocoronene/sto3g/est_basis/hexabenzocorornene_faraday_discussion.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arnab/arnab/workspace/2024_faraday_discussions_data/hexabenzocoronene/sto3g/est_basis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3918A143-2565-1848-B720-B834FEFA3BEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F725B23D-C308-F749-8A04-C03FA7FAC9DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1240" yWindow="760" windowWidth="29000" windowHeight="17920" xr2:uid="{FEE3860C-D3F4-C840-B97D-F5B8812B6184}"/>
+    <workbookView xWindow="32760" yWindow="500" windowWidth="38400" windowHeight="19560" activeTab="1" xr2:uid="{FEE3860C-D3F4-C840-B97D-F5B8812B6184}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -35,8 +36,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="64">
   <si>
     <t>Ecore</t>
   </si>
@@ -143,6 +166,9 @@
     <t>nb4</t>
   </si>
   <si>
+    <t>=</t>
+  </si>
+  <si>
     <t>&lt;N&gt;</t>
   </si>
   <si>
@@ -183,6 +209,48 @@
   </si>
   <si>
     <t>sto3g</t>
+  </si>
+  <si>
+    <t>Cov(NI,</t>
+  </si>
+  <si>
+    <t>NJ):</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>κ2(Sz)</t>
+  </si>
+  <si>
+    <t>*************************</t>
+  </si>
+  <si>
+    <t>Cov(SzI,</t>
+  </si>
+  <si>
+    <t>SzJ):</t>
+  </si>
+  <si>
+    <t>κ2(Q)</t>
+  </si>
+  <si>
+    <t>**************************</t>
+  </si>
+  <si>
+    <t>Cov(QI,</t>
+  </si>
+  <si>
+    <t>QJ):</t>
+  </si>
+  <si>
+    <t>7×7</t>
+  </si>
+  <si>
+    <t>Matrix{Float64}:</t>
+  </si>
+  <si>
+    <t>Cov(S2i,S2j):</t>
   </si>
 </sst>
 </file>
@@ -752,7 +820,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="189">
+  <cellXfs count="190">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -927,6 +995,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="37" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="37" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="20" fontId="38" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -2355,8 +2424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C7E9B32-CF8A-A644-91BD-4F75E173F94D}">
   <dimension ref="A1:AH234"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N80" zoomScale="50" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U110" sqref="U110"/>
+    <sheetView topLeftCell="A79" zoomScale="50" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M112" sqref="M112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -2525,26 +2594,26 @@
       <c r="T4" s="3"/>
       <c r="U4" s="3"/>
       <c r="V4" s="3"/>
-      <c r="AA4" s="178"/>
-      <c r="AB4" s="179">
+      <c r="AA4" s="179"/>
+      <c r="AB4" s="180">
         <v>1</v>
       </c>
-      <c r="AC4" s="179">
+      <c r="AC4" s="180">
         <v>2</v>
       </c>
-      <c r="AD4" s="179">
+      <c r="AD4" s="180">
         <v>3</v>
       </c>
-      <c r="AE4" s="179">
+      <c r="AE4" s="180">
         <v>4</v>
       </c>
-      <c r="AF4" s="179">
+      <c r="AF4" s="180">
         <v>5</v>
       </c>
-      <c r="AG4" s="179">
+      <c r="AG4" s="180">
         <v>6</v>
       </c>
-      <c r="AH4" s="179">
+      <c r="AH4" s="180">
         <v>7</v>
       </c>
     </row>
@@ -2591,31 +2660,31 @@
       <c r="T5" s="3"/>
       <c r="U5" s="3"/>
       <c r="V5" s="3"/>
-      <c r="W5" s="175"/>
-      <c r="X5" s="175"/>
-      <c r="Y5" s="176"/>
-      <c r="AA5" s="174" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB5" s="174">
+      <c r="W5" s="176"/>
+      <c r="X5" s="176"/>
+      <c r="Y5" s="177"/>
+      <c r="AA5" s="175" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB5" s="175">
         <v>6.0000432500000001</v>
       </c>
-      <c r="AC5" s="174">
+      <c r="AC5" s="175">
         <v>6.0000585400000004</v>
       </c>
-      <c r="AD5" s="174">
+      <c r="AD5" s="175">
         <v>6.0000649199999998</v>
       </c>
-      <c r="AE5" s="174">
+      <c r="AE5" s="175">
         <v>6.0000470000000004</v>
       </c>
-      <c r="AF5" s="174">
+      <c r="AF5" s="175">
         <v>6.0000588300000004</v>
       </c>
-      <c r="AG5" s="174">
+      <c r="AG5" s="175">
         <v>6.00005963</v>
       </c>
-      <c r="AH5" s="174">
+      <c r="AH5" s="175">
         <v>5.9996678299999999</v>
       </c>
     </row>
@@ -2646,31 +2715,31 @@
       <c r="T6" s="3"/>
       <c r="U6" s="3"/>
       <c r="V6" s="3"/>
-      <c r="W6" s="175"/>
-      <c r="X6" s="175"/>
-      <c r="Y6" s="177"/>
-      <c r="AA6" s="174" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB6" s="174">
+      <c r="W6" s="176"/>
+      <c r="X6" s="176"/>
+      <c r="Y6" s="178"/>
+      <c r="AA6" s="175" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB6" s="175">
         <v>2.08E-6</v>
       </c>
-      <c r="AC6" s="174">
+      <c r="AC6" s="175">
         <v>6.1E-6</v>
       </c>
-      <c r="AD6" s="174">
+      <c r="AD6" s="175">
         <v>-3.1E-7</v>
       </c>
-      <c r="AE6" s="174">
+      <c r="AE6" s="175">
         <v>5.48E-6</v>
       </c>
-      <c r="AF6" s="174">
+      <c r="AF6" s="175">
         <v>7.3300000000000001E-6</v>
       </c>
-      <c r="AG6" s="174">
+      <c r="AG6" s="175">
         <v>4.4999999999999998E-7</v>
       </c>
-      <c r="AH6" s="174">
+      <c r="AH6" s="175">
         <v>-2.1129999999999999E-5</v>
       </c>
     </row>
@@ -2716,31 +2785,31 @@
       <c r="T7" s="3"/>
       <c r="U7" s="3"/>
       <c r="V7" s="3"/>
-      <c r="W7" s="175"/>
-      <c r="X7" s="175"/>
-      <c r="Y7" s="177"/>
-      <c r="AA7" s="174" t="s">
-        <v>37</v>
-      </c>
-      <c r="AB7" s="174">
+      <c r="W7" s="176"/>
+      <c r="X7" s="176"/>
+      <c r="Y7" s="178"/>
+      <c r="AA7" s="175" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB7" s="175">
         <v>3.8133779999999999E-2</v>
       </c>
-      <c r="AC7" s="174">
+      <c r="AC7" s="175">
         <v>3.8136339999999998E-2</v>
       </c>
-      <c r="AD7" s="174">
+      <c r="AD7" s="175">
         <v>3.8366869999999997E-2</v>
       </c>
-      <c r="AE7" s="174">
+      <c r="AE7" s="175">
         <v>3.81255E-2</v>
       </c>
-      <c r="AF7" s="174">
+      <c r="AF7" s="175">
         <v>3.8141479999999998E-2</v>
       </c>
-      <c r="AG7" s="174">
+      <c r="AG7" s="175">
         <v>3.8380020000000001E-2</v>
       </c>
-      <c r="AH7" s="174">
+      <c r="AH7" s="175">
         <v>8.5687390000000002E-2</v>
       </c>
     </row>
@@ -2783,31 +2852,31 @@
       <c r="T8" s="3"/>
       <c r="U8" s="3"/>
       <c r="V8" s="3"/>
-      <c r="W8" s="175"/>
-      <c r="X8" s="175"/>
-      <c r="Y8" s="177"/>
-      <c r="AA8" s="174" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB8" s="174">
+      <c r="W8" s="176"/>
+      <c r="X8" s="176"/>
+      <c r="Y8" s="178"/>
+      <c r="AA8" s="175" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB8" s="175">
         <v>-27.75210843</v>
       </c>
-      <c r="AC8" s="174">
+      <c r="AC8" s="175">
         <v>-27.752177280000002</v>
       </c>
-      <c r="AD8" s="174">
+      <c r="AD8" s="175">
         <v>-27.75198722</v>
       </c>
-      <c r="AE8" s="174">
+      <c r="AE8" s="175">
         <v>-27.75212509</v>
       </c>
-      <c r="AF8" s="174">
+      <c r="AF8" s="175">
         <v>-27.752173519999999</v>
       </c>
-      <c r="AG8" s="174">
+      <c r="AG8" s="175">
         <v>-27.75195523</v>
       </c>
-      <c r="AH8" s="174">
+      <c r="AH8" s="175">
         <v>-34.042855969999998</v>
       </c>
     </row>
@@ -2860,31 +2929,31 @@
       <c r="T9" s="3"/>
       <c r="U9" s="3"/>
       <c r="V9" s="3"/>
-      <c r="W9" s="175"/>
-      <c r="X9" s="175"/>
-      <c r="Y9" s="177"/>
-      <c r="AA9" s="174" t="s">
-        <v>39</v>
-      </c>
-      <c r="AB9" s="174">
+      <c r="W9" s="176"/>
+      <c r="X9" s="176"/>
+      <c r="Y9" s="178"/>
+      <c r="AA9" s="175" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB9" s="175">
         <v>-6.3503054199999998</v>
       </c>
-      <c r="AC9" s="174">
+      <c r="AC9" s="175">
         <v>-6.3503062999999997</v>
       </c>
-      <c r="AD9" s="174">
+      <c r="AD9" s="175">
         <v>-6.3502019399999998</v>
       </c>
-      <c r="AE9" s="174">
+      <c r="AE9" s="175">
         <v>-6.3503078000000004</v>
       </c>
-      <c r="AF9" s="174">
+      <c r="AF9" s="175">
         <v>-6.35030216</v>
       </c>
-      <c r="AG9" s="174">
+      <c r="AG9" s="175">
         <v>-6.3501975499999999</v>
       </c>
-      <c r="AH9" s="174">
+      <c r="AH9" s="175">
         <v>-6.23124638</v>
       </c>
     </row>
@@ -5534,12 +5603,12 @@
     </row>
     <row r="94" spans="6:18" ht="34">
       <c r="F94" s="103"/>
-      <c r="H94" s="187" t="s">
-        <v>48</v>
-      </c>
-      <c r="I94" s="185"/>
-      <c r="J94" s="185"/>
-      <c r="K94" s="185"/>
+      <c r="H94" s="188" t="s">
+        <v>49</v>
+      </c>
+      <c r="I94" s="186"/>
+      <c r="J94" s="186"/>
+      <c r="K94" s="186"/>
       <c r="L94" s="101"/>
       <c r="M94" s="101"/>
       <c r="N94" s="101"/>
@@ -5548,10 +5617,10 @@
     </row>
     <row r="95" spans="6:18" ht="34">
       <c r="F95" s="103"/>
-      <c r="H95" s="185"/>
-      <c r="I95" s="185"/>
-      <c r="J95" s="185"/>
-      <c r="K95" s="185"/>
+      <c r="H95" s="186"/>
+      <c r="I95" s="186"/>
+      <c r="J95" s="186"/>
+      <c r="K95" s="186"/>
       <c r="L95" s="101"/>
       <c r="M95" s="101"/>
       <c r="N95" s="101"/>
@@ -5560,15 +5629,15 @@
     </row>
     <row r="96" spans="6:18" ht="34">
       <c r="F96" s="103"/>
-      <c r="H96" s="185"/>
-      <c r="I96" s="185" t="s">
+      <c r="H96" s="186"/>
+      <c r="I96" s="186" t="s">
         <v>12</v>
       </c>
-      <c r="J96" s="185" t="s">
-        <v>40</v>
-      </c>
-      <c r="K96" s="185" t="s">
+      <c r="J96" s="186" t="s">
         <v>41</v>
+      </c>
+      <c r="K96" s="186" t="s">
+        <v>42</v>
       </c>
       <c r="L96" s="101"/>
       <c r="M96" s="101"/>
@@ -5578,82 +5647,111 @@
     </row>
     <row r="97" spans="6:18" ht="34">
       <c r="F97" s="103"/>
-      <c r="H97" s="185"/>
-      <c r="I97" s="186">
+      <c r="H97" s="186"/>
+      <c r="I97" s="187">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="J97" s="185">
+      <c r="J97" s="186">
         <v>-1582.4262381000001</v>
       </c>
-      <c r="K97" s="185">
+      <c r="K97" s="186">
         <v>-1582.4398933300001</v>
       </c>
-      <c r="L97" s="188">
+      <c r="L97" s="189">
         <v>6534</v>
       </c>
-      <c r="M97" s="101"/>
-      <c r="N97" s="101"/>
-      <c r="O97" s="101"/>
+      <c r="M97" s="101">
+        <f>(K97-J97)</f>
+        <v>-1.3655230000040319E-2</v>
+      </c>
+      <c r="N97" s="101" cm="1">
+        <f t="array" ref="N97:O101">LINEST(J97:J100,M97:M100,TRUE,TRUE)</f>
+        <v>-1.7240834151147555</v>
+      </c>
+      <c r="O97" s="101">
+        <v>-1582.4497914351882</v>
+      </c>
       <c r="R97" s="101"/>
     </row>
     <row r="98" spans="6:18" ht="34">
       <c r="F98" s="103"/>
-      <c r="H98" s="185"/>
-      <c r="I98" s="186">
+      <c r="H98" s="186"/>
+      <c r="I98" s="187">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="J98" s="185">
+      <c r="J98" s="186">
         <v>-1582.4278953200001</v>
       </c>
-      <c r="K98" s="185">
+      <c r="K98" s="186">
         <v>-1582.4405839000001</v>
       </c>
-      <c r="L98" s="188">
+      <c r="L98" s="189">
         <v>9870</v>
       </c>
-      <c r="M98" s="101"/>
-      <c r="N98" s="101"/>
-      <c r="O98" s="101"/>
+      <c r="M98" s="101">
+        <f t="shared" ref="M98:M100" si="15">(K98-J98)</f>
+        <v>-1.2688580000030925E-2</v>
+      </c>
+      <c r="N98" s="101">
+        <v>1.6485000903880907E-2</v>
+      </c>
+      <c r="O98" s="101">
+        <v>1.9655507781928154E-4</v>
+      </c>
       <c r="R98" s="101"/>
     </row>
     <row r="99" spans="6:18" ht="34">
       <c r="F99" s="103"/>
-      <c r="H99" s="185"/>
-      <c r="I99" s="186">
+      <c r="H99" s="186"/>
+      <c r="I99" s="187">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="J99" s="185">
+      <c r="J99" s="186">
         <v>-1582.43029069</v>
       </c>
-      <c r="K99" s="185">
+      <c r="K99" s="186">
         <v>-1582.4416363600001</v>
       </c>
-      <c r="L99" s="188">
+      <c r="L99" s="189">
         <v>19285</v>
       </c>
-      <c r="M99" s="101"/>
-      <c r="N99" s="101"/>
-      <c r="O99" s="101"/>
+      <c r="M99" s="101">
+        <f t="shared" si="15"/>
+        <v>-1.1345670000082464E-2</v>
+      </c>
+      <c r="N99" s="101">
+        <v>0.99981718492915517</v>
+      </c>
+      <c r="O99" s="101">
+        <v>5.0014794009371869E-5</v>
+      </c>
       <c r="R99" s="101"/>
     </row>
     <row r="100" spans="6:18" ht="34">
       <c r="F100" s="103"/>
-      <c r="H100" s="185"/>
-      <c r="I100" s="186">
+      <c r="H100" s="186"/>
+      <c r="I100" s="187">
         <v>2.5000000000000001E-4</v>
       </c>
-      <c r="J100" s="185">
+      <c r="J100" s="186">
         <v>-1582.4331830200001</v>
       </c>
-      <c r="K100" s="185">
+      <c r="K100" s="186">
         <v>-1582.4427990300001</v>
       </c>
-      <c r="L100" s="188">
+      <c r="L100" s="189">
         <v>58969</v>
       </c>
-      <c r="M100" s="101"/>
-      <c r="N100" s="101"/>
-      <c r="O100" s="101"/>
+      <c r="M100" s="101">
+        <f t="shared" si="15"/>
+        <v>-9.6160099999451631E-3</v>
+      </c>
+      <c r="N100" s="101">
+        <v>10938.017093545897</v>
+      </c>
+      <c r="O100" s="101">
+        <v>2</v>
+      </c>
       <c r="R100" s="101"/>
     </row>
     <row r="101" spans="6:18" ht="29">
@@ -5664,8 +5762,12 @@
       <c r="K101" s="101"/>
       <c r="L101" s="101"/>
       <c r="M101" s="101"/>
-      <c r="N101" s="101"/>
-      <c r="O101" s="101"/>
+      <c r="N101" s="101">
+        <v>2.7361226840528001E-5</v>
+      </c>
+      <c r="O101" s="101">
+        <v>5.0029592395998007E-9</v>
+      </c>
       <c r="R101" s="101"/>
     </row>
     <row r="102" spans="6:18" ht="29">
@@ -5702,199 +5804,240 @@
     </row>
     <row r="105" spans="6:18" ht="32">
       <c r="F105" s="103"/>
-      <c r="H105" s="180" t="s">
+      <c r="H105" s="181" t="s">
         <v>1</v>
       </c>
-      <c r="I105" s="180"/>
-      <c r="J105" s="180"/>
-      <c r="K105" s="180"/>
-      <c r="L105" s="180"/>
-      <c r="M105" s="180"/>
+      <c r="I105" s="181"/>
+      <c r="J105" s="181"/>
+      <c r="K105" s="181"/>
+      <c r="L105" s="181"/>
+      <c r="M105" s="181"/>
       <c r="N105" s="101"/>
       <c r="O105" s="101"/>
       <c r="R105" s="101"/>
     </row>
     <row r="106" spans="6:18" ht="32">
       <c r="F106" s="103"/>
-      <c r="H106" s="181"/>
-      <c r="I106" s="181"/>
-      <c r="J106" s="181"/>
-      <c r="K106" s="181"/>
-      <c r="L106" s="181"/>
-      <c r="M106" s="180"/>
+      <c r="H106" s="182"/>
+      <c r="I106" s="182"/>
+      <c r="J106" s="182"/>
+      <c r="K106" s="182"/>
+      <c r="L106" s="182"/>
+      <c r="M106" s="181"/>
       <c r="N106" s="101"/>
       <c r="O106" s="101"/>
       <c r="R106" s="101"/>
     </row>
     <row r="107" spans="6:18" ht="32">
       <c r="F107" s="103"/>
-      <c r="H107" s="181" t="s">
-        <v>44</v>
-      </c>
-      <c r="I107" s="182">
+      <c r="H107" s="182" t="s">
+        <v>45</v>
+      </c>
+      <c r="I107" s="183">
         <v>-1479.3366410466199</v>
       </c>
-      <c r="J107" s="181"/>
-      <c r="K107" s="181"/>
-      <c r="L107" s="180"/>
-      <c r="M107" s="180"/>
+      <c r="J107" s="182"/>
+      <c r="K107" s="182"/>
+      <c r="L107" s="181"/>
+      <c r="M107" s="181"/>
       <c r="N107" s="101"/>
       <c r="O107" s="101"/>
       <c r="R107" s="101"/>
     </row>
     <row r="108" spans="6:18" ht="31">
       <c r="F108" s="103"/>
-      <c r="H108" s="183" t="s">
+      <c r="H108" s="184" t="s">
+        <v>43</v>
+      </c>
+      <c r="I108" s="184" t="s">
+        <v>46</v>
+      </c>
+      <c r="J108" s="184" t="s">
+        <v>41</v>
+      </c>
+      <c r="K108" s="184" t="s">
+        <v>47</v>
+      </c>
+      <c r="L108" s="184" t="s">
         <v>42</v>
       </c>
-      <c r="I108" s="183" t="s">
-        <v>45</v>
-      </c>
-      <c r="J108" s="183" t="s">
-        <v>40</v>
-      </c>
-      <c r="K108" s="183" t="s">
-        <v>46</v>
-      </c>
-      <c r="L108" s="183" t="s">
-        <v>41</v>
-      </c>
-      <c r="M108" s="183" t="s">
-        <v>47</v>
+      <c r="M108" s="184" t="s">
+        <v>48</v>
       </c>
       <c r="N108" s="101"/>
       <c r="O108" s="101"/>
       <c r="R108" s="101"/>
     </row>
-    <row r="109" spans="6:18" ht="31">
+    <row r="109" spans="6:18" ht="32">
       <c r="F109" s="103"/>
-      <c r="H109" s="184">
+      <c r="H109" s="185">
         <v>1E-3</v>
       </c>
-      <c r="I109" s="183">
+      <c r="I109" s="184">
         <v>-122.33863101999999</v>
       </c>
-      <c r="J109" s="183">
+      <c r="J109" s="184">
         <f>(I109+I107)</f>
         <v>-1601.67527206662</v>
       </c>
-      <c r="K109" s="183">
+      <c r="K109" s="184">
         <v>-122.35207265</v>
       </c>
-      <c r="L109" s="183">
+      <c r="L109" s="184">
         <f>(K109-1479.336641)</f>
         <v>-1601.6887136500002</v>
       </c>
-      <c r="M109" s="183">
+      <c r="M109" s="184">
         <v>5777</v>
       </c>
-      <c r="N109" s="101"/>
-      <c r="O109" s="101"/>
+      <c r="N109" s="101">
+        <f>L109-J109</f>
+        <v>-1.3441583380199518E-2</v>
+      </c>
+      <c r="O109" s="173" cm="1">
+        <f t="array" ref="O109:P113">LINEST(J109:J113,N109:N113,TRUE,TRUE)</f>
+        <v>-1.5864826117804571</v>
+      </c>
+      <c r="P109" s="173">
+        <v>-1601.6966147744274</v>
+      </c>
       <c r="R109" s="101"/>
     </row>
-    <row r="110" spans="6:18" ht="31">
+    <row r="110" spans="6:18" ht="32">
       <c r="F110" s="103"/>
-      <c r="H110" s="184">
+      <c r="H110" s="185">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="I110" s="183">
+      <c r="I110" s="184">
         <v>-122.33992397</v>
       </c>
-      <c r="J110" s="183">
+      <c r="J110" s="184">
         <f>(I110-1479.336641)</f>
         <v>-1601.6765649700001</v>
       </c>
-      <c r="K110" s="183">
+      <c r="K110" s="184">
         <v>-122.3525685</v>
       </c>
-      <c r="L110" s="183">
-        <f t="shared" ref="L110:L113" si="15">(K110-1479.336641)</f>
+      <c r="L110" s="184">
+        <f t="shared" ref="L110:L113" si="16">(K110-1479.336641)</f>
         <v>-1601.6892095000001</v>
       </c>
-      <c r="M110" s="183">
+      <c r="M110" s="184">
         <v>7490</v>
       </c>
-      <c r="N110" s="101"/>
-      <c r="O110" s="101"/>
+      <c r="N110" s="101">
+        <f t="shared" ref="N110:N113" si="17">L110-J110</f>
+        <v>-1.2644529999988663E-2</v>
+      </c>
+      <c r="O110" s="173">
+        <v>6.6657794249401795E-3</v>
+      </c>
+      <c r="P110" s="173">
+        <v>7.7155466377196969E-5</v>
+      </c>
       <c r="R110" s="101"/>
     </row>
-    <row r="111" spans="6:18" ht="31">
+    <row r="111" spans="6:18" ht="32">
       <c r="F111" s="103"/>
-      <c r="H111" s="184">
+      <c r="H111" s="185">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="I111" s="183">
+      <c r="I111" s="184">
         <v>-122.34141757</v>
       </c>
-      <c r="J111" s="183">
-        <f t="shared" ref="J111:J113" si="16">(I111-1479.336641)</f>
+      <c r="J111" s="184">
+        <f t="shared" ref="J111:J113" si="18">(I111-1479.336641)</f>
         <v>-1601.6780585700001</v>
       </c>
-      <c r="K111" s="183">
+      <c r="K111" s="184">
         <v>-122.35311428999999</v>
       </c>
-      <c r="L111" s="183">
-        <f t="shared" si="15"/>
+      <c r="L111" s="184">
+        <f t="shared" si="16"/>
         <v>-1601.68975529</v>
       </c>
-      <c r="M111" s="183">
+      <c r="M111" s="184">
         <v>10688</v>
       </c>
-      <c r="N111" s="101"/>
-      <c r="O111" s="101"/>
+      <c r="N111" s="101">
+        <f t="shared" si="17"/>
+        <v>-1.1696719999918059E-2</v>
+      </c>
+      <c r="O111" s="173">
+        <v>0.99994704225320441</v>
+      </c>
+      <c r="P111" s="173">
+        <v>2.3118542811312708E-5</v>
+      </c>
       <c r="R111" s="101"/>
     </row>
-    <row r="112" spans="6:18" ht="31">
+    <row r="112" spans="6:18" ht="32">
       <c r="F112" s="103"/>
-      <c r="H112" s="184">
+      <c r="H112" s="185">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="I112" s="183">
+      <c r="I112" s="184">
         <v>-122.34333904</v>
       </c>
-      <c r="J112" s="183">
+      <c r="J112" s="184">
+        <f t="shared" si="18"/>
+        <v>-1601.6799800400001</v>
+      </c>
+      <c r="K112" s="184">
+        <v>-122.35384162</v>
+      </c>
+      <c r="L112" s="184">
         <f t="shared" si="16"/>
-        <v>-1601.6799800400001</v>
-      </c>
-      <c r="K112" s="183">
-        <v>-122.35384162</v>
-      </c>
-      <c r="L112" s="183">
-        <f t="shared" si="15"/>
         <v>-1601.69048262</v>
       </c>
-      <c r="M112" s="183">
+      <c r="M112" s="184">
         <v>18501</v>
       </c>
-      <c r="N112" s="101"/>
-      <c r="O112" s="101"/>
+      <c r="N112" s="101">
+        <f t="shared" si="17"/>
+        <v>-1.0502579999865702E-2</v>
+      </c>
+      <c r="O112" s="173">
+        <v>56645.935831400689</v>
+      </c>
+      <c r="P112" s="173">
+        <v>3</v>
+      </c>
       <c r="R112" s="101"/>
     </row>
-    <row r="113" spans="6:20" ht="31">
+    <row r="113" spans="6:20" ht="32">
       <c r="F113" s="103"/>
-      <c r="H113" s="184">
+      <c r="H113" s="185">
         <v>2.5000000000000001E-4</v>
       </c>
-      <c r="I113" s="183">
+      <c r="I113" s="184">
         <f>-122.34556873</f>
         <v>-122.34556873</v>
       </c>
-      <c r="J113" s="183">
+      <c r="J113" s="184">
+        <f t="shared" si="18"/>
+        <v>-1601.6822097300001</v>
+      </c>
+      <c r="K113" s="184">
+        <v>-122.35463566</v>
+      </c>
+      <c r="L113" s="184">
         <f t="shared" si="16"/>
-        <v>-1601.6822097300001</v>
-      </c>
-      <c r="K113" s="183">
-        <v>-122.35463566</v>
-      </c>
-      <c r="L113" s="183">
-        <f t="shared" si="15"/>
         <v>-1601.6912766600001</v>
       </c>
-      <c r="M113" s="183">
+      <c r="M113" s="184">
         <v>56900</v>
       </c>
-      <c r="N113" s="101"/>
-      <c r="O113" s="101"/>
+      <c r="N113" s="101">
+        <f t="shared" si="17"/>
+        <v>-9.066930000017237E-3</v>
+      </c>
+      <c r="O113" s="173">
+        <v>3.02753846162659E-5</v>
+      </c>
+      <c r="P113" s="173">
+        <v>1.6034010651554952E-9</v>
+      </c>
       <c r="R113" s="101"/>
     </row>
     <row r="114" spans="6:20" ht="29">
@@ -5924,34 +6067,34 @@
     <row r="116" spans="6:20" ht="29">
       <c r="F116" s="103"/>
       <c r="H116" s="101" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I116" s="101" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J116" s="101" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K116" s="101" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L116" s="101" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="M116" s="101" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N116" s="101" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="O116" s="101" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="P116" s="101" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Q116" s="101" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="R116" s="101"/>
     </row>
@@ -6952,4 +7095,1300 @@
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14D539C4-92C5-7D4D-B7A9-0DE6F6AFF58C}">
+  <dimension ref="A1:Q46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M31" sqref="M31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:17">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="174">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1">
+        <v>1</v>
+      </c>
+      <c r="L1">
+        <v>2</v>
+      </c>
+      <c r="M1">
+        <v>6</v>
+      </c>
+      <c r="N1">
+        <v>3</v>
+      </c>
+      <c r="O1">
+        <v>5</v>
+      </c>
+      <c r="P1">
+        <v>7</v>
+      </c>
+      <c r="Q1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="B2">
+        <v>2.1100899999999999E-2</v>
+      </c>
+      <c r="C2">
+        <v>-6.33257E-3</v>
+      </c>
+      <c r="D2">
+        <v>-1.1367E-4</v>
+      </c>
+      <c r="E2">
+        <v>-2.4528000000000001E-4</v>
+      </c>
+      <c r="F2">
+        <v>-1.1387000000000001E-4</v>
+      </c>
+      <c r="G2">
+        <v>-6.3035399999999998E-3</v>
+      </c>
+      <c r="H2">
+        <v>-7.9919699999999993E-3</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>3.1516389999999998E-2</v>
+      </c>
+      <c r="L2">
+        <v>8.8222800000000001E-3</v>
+      </c>
+      <c r="M2">
+        <v>8.7888900000000006E-3</v>
+      </c>
+      <c r="N2">
+        <v>-2.2436E-4</v>
+      </c>
+      <c r="O2">
+        <v>-2.2005000000000001E-4</v>
+      </c>
+      <c r="P2">
+        <v>1.099497E-2</v>
+      </c>
+      <c r="Q2">
+        <v>-4.0444999999999999E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="B3">
+        <v>-6.33257E-3</v>
+      </c>
+      <c r="C3">
+        <v>2.109258E-2</v>
+      </c>
+      <c r="D3">
+        <v>-6.3041E-3</v>
+      </c>
+      <c r="E3">
+        <v>-1.1387000000000001E-4</v>
+      </c>
+      <c r="F3">
+        <v>-2.4444000000000001E-4</v>
+      </c>
+      <c r="G3">
+        <v>-1.1378E-4</v>
+      </c>
+      <c r="H3">
+        <v>-7.9838200000000008E-3</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>8.8222800000000001E-3</v>
+      </c>
+      <c r="L3">
+        <v>3.1507840000000002E-2</v>
+      </c>
+      <c r="M3">
+        <v>-2.2440000000000001E-4</v>
+      </c>
+      <c r="N3">
+        <v>8.7883500000000003E-3</v>
+      </c>
+      <c r="O3">
+        <v>-4.0474E-4</v>
+      </c>
+      <c r="P3">
+        <v>1.09871E-2</v>
+      </c>
+      <c r="Q3">
+        <v>-2.2006E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="B4">
+        <v>-1.1367E-4</v>
+      </c>
+      <c r="C4">
+        <v>-6.3041E-3</v>
+      </c>
+      <c r="D4">
+        <v>2.1166230000000001E-2</v>
+      </c>
+      <c r="E4">
+        <v>-6.30352E-3</v>
+      </c>
+      <c r="F4">
+        <v>-1.1378E-4</v>
+      </c>
+      <c r="G4">
+        <v>-2.5287999999999998E-4</v>
+      </c>
+      <c r="H4">
+        <v>-8.0782700000000002E-3</v>
+      </c>
+      <c r="J4">
+        <v>6</v>
+      </c>
+      <c r="K4">
+        <v>8.7888900000000006E-3</v>
+      </c>
+      <c r="L4">
+        <v>-2.2440000000000001E-4</v>
+      </c>
+      <c r="M4">
+        <v>3.1591710000000002E-2</v>
+      </c>
+      <c r="N4">
+        <v>-3.6916E-4</v>
+      </c>
+      <c r="O4">
+        <v>8.7883000000000006E-3</v>
+      </c>
+      <c r="P4">
+        <v>1.1084999999999999E-2</v>
+      </c>
+      <c r="Q4">
+        <v>-2.2437999999999999E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="B5">
+        <v>-2.4528000000000001E-4</v>
+      </c>
+      <c r="C5">
+        <v>-1.1387000000000001E-4</v>
+      </c>
+      <c r="D5">
+        <v>-6.30352E-3</v>
+      </c>
+      <c r="E5">
+        <v>2.110091E-2</v>
+      </c>
+      <c r="F5">
+        <v>-6.33257E-3</v>
+      </c>
+      <c r="G5">
+        <v>-1.1367E-4</v>
+      </c>
+      <c r="H5">
+        <v>-7.9920100000000008E-3</v>
+      </c>
+      <c r="J5">
+        <v>3</v>
+      </c>
+      <c r="K5">
+        <v>-2.2436E-4</v>
+      </c>
+      <c r="L5">
+        <v>8.7883500000000003E-3</v>
+      </c>
+      <c r="M5">
+        <v>-3.6916E-4</v>
+      </c>
+      <c r="N5">
+        <v>3.1591269999999998E-2</v>
+      </c>
+      <c r="O5">
+        <v>-2.2437999999999999E-4</v>
+      </c>
+      <c r="P5">
+        <v>1.108454E-2</v>
+      </c>
+      <c r="Q5">
+        <v>8.7886400000000003E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="B6">
+        <v>-1.1387000000000001E-4</v>
+      </c>
+      <c r="C6">
+        <v>-2.4444000000000001E-4</v>
+      </c>
+      <c r="D6">
+        <v>-1.1378E-4</v>
+      </c>
+      <c r="E6">
+        <v>-6.33257E-3</v>
+      </c>
+      <c r="F6">
+        <v>2.1092610000000001E-2</v>
+      </c>
+      <c r="G6">
+        <v>-6.30409E-3</v>
+      </c>
+      <c r="H6">
+        <v>-7.9838700000000005E-3</v>
+      </c>
+      <c r="J6">
+        <v>5</v>
+      </c>
+      <c r="K6">
+        <v>-2.2005000000000001E-4</v>
+      </c>
+      <c r="L6">
+        <v>-4.0474E-4</v>
+      </c>
+      <c r="M6">
+        <v>8.7883000000000006E-3</v>
+      </c>
+      <c r="N6">
+        <v>-2.2437999999999999E-4</v>
+      </c>
+      <c r="O6">
+        <v>3.150787E-2</v>
+      </c>
+      <c r="P6">
+        <v>1.0987149999999999E-2</v>
+      </c>
+      <c r="Q6">
+        <v>8.8223299999999998E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="B7">
+        <v>-6.3035399999999998E-3</v>
+      </c>
+      <c r="C7">
+        <v>-1.1378E-4</v>
+      </c>
+      <c r="D7">
+        <v>-2.5287999999999998E-4</v>
+      </c>
+      <c r="E7">
+        <v>-1.1367E-4</v>
+      </c>
+      <c r="F7">
+        <v>-6.30409E-3</v>
+      </c>
+      <c r="G7">
+        <v>2.1166730000000002E-2</v>
+      </c>
+      <c r="H7">
+        <v>-8.0787600000000008E-3</v>
+      </c>
+      <c r="J7">
+        <v>7</v>
+      </c>
+      <c r="K7">
+        <v>1.099497E-2</v>
+      </c>
+      <c r="L7">
+        <v>1.09871E-2</v>
+      </c>
+      <c r="M7">
+        <v>1.1084999999999999E-2</v>
+      </c>
+      <c r="N7">
+        <v>1.108454E-2</v>
+      </c>
+      <c r="O7">
+        <v>1.0987149999999999E-2</v>
+      </c>
+      <c r="P7">
+        <v>5.8237990000000003E-2</v>
+      </c>
+      <c r="Q7">
+        <v>1.0995069999999999E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="B8">
+        <v>-7.9919699999999993E-3</v>
+      </c>
+      <c r="C8">
+        <v>-7.9838200000000008E-3</v>
+      </c>
+      <c r="D8">
+        <v>-8.0782700000000002E-3</v>
+      </c>
+      <c r="E8">
+        <v>-7.9920100000000008E-3</v>
+      </c>
+      <c r="F8">
+        <v>-7.9838700000000005E-3</v>
+      </c>
+      <c r="G8">
+        <v>-8.0787600000000008E-3</v>
+      </c>
+      <c r="H8">
+        <v>4.8108690000000003E-2</v>
+      </c>
+      <c r="J8">
+        <v>4</v>
+      </c>
+      <c r="K8">
+        <v>-4.0444999999999999E-4</v>
+      </c>
+      <c r="L8">
+        <v>-2.2006E-4</v>
+      </c>
+      <c r="M8">
+        <v>-2.2437999999999999E-4</v>
+      </c>
+      <c r="N8">
+        <v>8.7886400000000003E-3</v>
+      </c>
+      <c r="O8">
+        <v>8.8223299999999998E-3</v>
+      </c>
+      <c r="P8">
+        <v>1.0995069999999999E-2</v>
+      </c>
+      <c r="Q8">
+        <v>3.1516019999999999E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="B10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="174">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="B12">
+        <v>7.4845500000000004E-3</v>
+      </c>
+      <c r="C12">
+        <v>-2.2620000000000001E-3</v>
+      </c>
+      <c r="D12">
+        <v>-3.294E-5</v>
+      </c>
+      <c r="E12">
+        <v>-8.3369999999999996E-5</v>
+      </c>
+      <c r="F12">
+        <v>-3.3160000000000001E-5</v>
+      </c>
+      <c r="G12">
+        <v>-3.2539999999999997E-5</v>
+      </c>
+      <c r="H12">
+        <v>-2.8255899999999998E-3</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>2</v>
+      </c>
+      <c r="M12">
+        <v>3</v>
+      </c>
+      <c r="N12">
+        <v>4</v>
+      </c>
+      <c r="O12">
+        <v>5</v>
+      </c>
+      <c r="P12">
+        <v>6</v>
+      </c>
+      <c r="Q12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="B13">
+        <v>-2.2620000000000001E-3</v>
+      </c>
+      <c r="C13">
+        <v>7.4815100000000002E-3</v>
+      </c>
+      <c r="D13">
+        <v>-2.24727E-3</v>
+      </c>
+      <c r="E13">
+        <v>-3.3160000000000001E-5</v>
+      </c>
+      <c r="F13">
+        <v>-8.3120000000000004E-5</v>
+      </c>
+      <c r="G13">
+        <v>-3.2539999999999997E-5</v>
+      </c>
+      <c r="H13">
+        <v>-2.82343E-3</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>3.1516389999999998E-2</v>
+      </c>
+      <c r="L13">
+        <v>8.8222800000000001E-3</v>
+      </c>
+      <c r="M13">
+        <v>-2.2436E-4</v>
+      </c>
+      <c r="N13">
+        <v>-4.0444999999999999E-4</v>
+      </c>
+      <c r="O13">
+        <v>-2.2005000000000001E-4</v>
+      </c>
+      <c r="P13">
+        <v>8.7888900000000006E-3</v>
+      </c>
+      <c r="Q13">
+        <v>1.099497E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="B14">
+        <v>-3.294E-5</v>
+      </c>
+      <c r="C14">
+        <v>-2.24727E-3</v>
+      </c>
+      <c r="D14">
+        <v>7.5042800000000003E-3</v>
+      </c>
+      <c r="E14">
+        <v>-2.24749E-3</v>
+      </c>
+      <c r="F14">
+        <v>-3.2539999999999997E-5</v>
+      </c>
+      <c r="G14">
+        <v>-8.8189999999999994E-5</v>
+      </c>
+      <c r="H14">
+        <v>-2.8558500000000001E-3</v>
+      </c>
+      <c r="J14">
+        <v>2</v>
+      </c>
+      <c r="K14">
+        <v>8.8222800000000001E-3</v>
+      </c>
+      <c r="L14">
+        <v>3.1507840000000002E-2</v>
+      </c>
+      <c r="M14">
+        <v>8.7883500000000003E-3</v>
+      </c>
+      <c r="N14">
+        <v>-2.2006E-4</v>
+      </c>
+      <c r="O14">
+        <v>-4.0474E-4</v>
+      </c>
+      <c r="P14">
+        <v>-2.2440000000000001E-4</v>
+      </c>
+      <c r="Q14">
+        <v>1.09871E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="B15">
+        <v>-8.3369999999999996E-5</v>
+      </c>
+      <c r="C15">
+        <v>-8.3369999999999996E-5</v>
+      </c>
+      <c r="D15">
+        <v>-2.24749E-3</v>
+      </c>
+      <c r="E15">
+        <v>7.4845600000000003E-3</v>
+      </c>
+      <c r="F15">
+        <v>-2.2619900000000002E-3</v>
+      </c>
+      <c r="G15">
+        <v>-3.294E-5</v>
+      </c>
+      <c r="H15">
+        <v>-2.8256000000000002E-3</v>
+      </c>
+      <c r="J15">
+        <v>3</v>
+      </c>
+      <c r="K15">
+        <v>-2.2436E-4</v>
+      </c>
+      <c r="L15">
+        <v>8.7883500000000003E-3</v>
+      </c>
+      <c r="M15">
+        <v>3.1591269999999998E-2</v>
+      </c>
+      <c r="N15">
+        <v>8.7886400000000003E-3</v>
+      </c>
+      <c r="O15">
+        <v>-2.2437999999999999E-4</v>
+      </c>
+      <c r="P15">
+        <v>-3.6916E-4</v>
+      </c>
+      <c r="Q15">
+        <v>1.108454E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="B16">
+        <v>-3.3160000000000001E-5</v>
+      </c>
+      <c r="C16">
+        <v>-3.3160000000000001E-5</v>
+      </c>
+      <c r="D16">
+        <v>-3.2539999999999997E-5</v>
+      </c>
+      <c r="E16">
+        <v>-2.2619900000000002E-3</v>
+      </c>
+      <c r="F16">
+        <v>7.4815100000000002E-3</v>
+      </c>
+      <c r="G16">
+        <v>-2.2472600000000001E-3</v>
+      </c>
+      <c r="H16">
+        <v>-2.82344E-3</v>
+      </c>
+      <c r="J16">
+        <v>4</v>
+      </c>
+      <c r="K16">
+        <v>-4.0444999999999999E-4</v>
+      </c>
+      <c r="L16">
+        <v>-2.2006E-4</v>
+      </c>
+      <c r="M16">
+        <v>8.7886400000000003E-3</v>
+      </c>
+      <c r="N16">
+        <v>3.1516019999999999E-2</v>
+      </c>
+      <c r="O16">
+        <v>8.8223299999999998E-3</v>
+      </c>
+      <c r="P16">
+        <v>-2.2437999999999999E-4</v>
+      </c>
+      <c r="Q16">
+        <v>1.0995069999999999E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
+      <c r="B17">
+        <v>-2.24749E-3</v>
+      </c>
+      <c r="C17">
+        <v>-3.2539999999999997E-5</v>
+      </c>
+      <c r="D17">
+        <v>-8.8189999999999994E-5</v>
+      </c>
+      <c r="E17">
+        <v>-3.294E-5</v>
+      </c>
+      <c r="F17">
+        <v>-2.2472600000000001E-3</v>
+      </c>
+      <c r="G17">
+        <v>7.5044100000000004E-3</v>
+      </c>
+      <c r="H17">
+        <v>-2.8559800000000002E-3</v>
+      </c>
+      <c r="J17">
+        <v>5</v>
+      </c>
+      <c r="K17">
+        <v>-2.2005000000000001E-4</v>
+      </c>
+      <c r="L17">
+        <v>-4.0474E-4</v>
+      </c>
+      <c r="M17">
+        <v>-2.2437999999999999E-4</v>
+      </c>
+      <c r="N17">
+        <v>8.8223299999999998E-3</v>
+      </c>
+      <c r="O17">
+        <v>3.150787E-2</v>
+      </c>
+      <c r="P17">
+        <v>8.7883000000000006E-3</v>
+      </c>
+      <c r="Q17">
+        <v>1.0987149999999999E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
+      <c r="B18">
+        <v>-2.8255899999999998E-3</v>
+      </c>
+      <c r="C18">
+        <v>-2.8255899999999998E-3</v>
+      </c>
+      <c r="D18">
+        <v>-2.8558500000000001E-3</v>
+      </c>
+      <c r="E18">
+        <v>-2.8256000000000002E-3</v>
+      </c>
+      <c r="F18">
+        <v>-2.82344E-3</v>
+      </c>
+      <c r="G18">
+        <v>-2.8559800000000002E-3</v>
+      </c>
+      <c r="H18">
+        <v>1.700989E-2</v>
+      </c>
+      <c r="J18">
+        <v>6</v>
+      </c>
+      <c r="K18">
+        <v>8.7888900000000006E-3</v>
+      </c>
+      <c r="L18">
+        <v>-2.2440000000000001E-4</v>
+      </c>
+      <c r="M18">
+        <v>-3.6916E-4</v>
+      </c>
+      <c r="N18">
+        <v>-2.2437999999999999E-4</v>
+      </c>
+      <c r="O18">
+        <v>8.7883000000000006E-3</v>
+      </c>
+      <c r="P18">
+        <v>3.1591710000000002E-2</v>
+      </c>
+      <c r="Q18">
+        <v>1.1084999999999999E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
+      <c r="J19">
+        <v>7</v>
+      </c>
+      <c r="K19">
+        <v>1.099497E-2</v>
+      </c>
+      <c r="L19">
+        <v>1.09871E-2</v>
+      </c>
+      <c r="M19">
+        <v>1.108454E-2</v>
+      </c>
+      <c r="N19">
+        <v>1.0995069999999999E-2</v>
+      </c>
+      <c r="O19">
+        <v>1.0987149999999999E-2</v>
+      </c>
+      <c r="P19">
+        <v>1.1084999999999999E-2</v>
+      </c>
+      <c r="Q19">
+        <v>5.8237990000000003E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="B20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
+      <c r="B21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="174">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E21" t="s">
+        <v>59</v>
+      </c>
+      <c r="F21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
+      <c r="B22">
+        <v>3.1516389999999998E-2</v>
+      </c>
+      <c r="C22">
+        <v>8.8222800000000001E-3</v>
+      </c>
+      <c r="D22">
+        <v>-2.2436E-4</v>
+      </c>
+      <c r="E22">
+        <v>-4.0444999999999999E-4</v>
+      </c>
+      <c r="F22">
+        <v>-2.2005000000000001E-4</v>
+      </c>
+      <c r="G22">
+        <v>8.7888900000000006E-3</v>
+      </c>
+      <c r="H22">
+        <v>1.099497E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
+      <c r="B23">
+        <v>8.8222800000000001E-3</v>
+      </c>
+      <c r="C23">
+        <v>3.1507840000000002E-2</v>
+      </c>
+      <c r="D23">
+        <v>8.7883500000000003E-3</v>
+      </c>
+      <c r="E23">
+        <v>-2.2006E-4</v>
+      </c>
+      <c r="F23">
+        <v>-4.0474E-4</v>
+      </c>
+      <c r="G23">
+        <v>-2.2440000000000001E-4</v>
+      </c>
+      <c r="H23">
+        <v>1.09871E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17">
+      <c r="B24">
+        <v>-2.2436E-4</v>
+      </c>
+      <c r="C24">
+        <v>8.7883500000000003E-3</v>
+      </c>
+      <c r="D24">
+        <v>3.1591269999999998E-2</v>
+      </c>
+      <c r="E24">
+        <v>8.7886400000000003E-3</v>
+      </c>
+      <c r="F24">
+        <v>-2.2437999999999999E-4</v>
+      </c>
+      <c r="G24">
+        <v>-3.6916E-4</v>
+      </c>
+      <c r="H24">
+        <v>1.108454E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
+      <c r="B25">
+        <v>-4.0444999999999999E-4</v>
+      </c>
+      <c r="C25">
+        <v>-2.2006E-4</v>
+      </c>
+      <c r="D25">
+        <v>8.7886400000000003E-3</v>
+      </c>
+      <c r="E25">
+        <v>3.1516019999999999E-2</v>
+      </c>
+      <c r="F25">
+        <v>8.8223299999999998E-3</v>
+      </c>
+      <c r="G25">
+        <v>-2.2437999999999999E-4</v>
+      </c>
+      <c r="H25">
+        <v>1.0995069999999999E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17">
+      <c r="B26">
+        <v>-2.2005000000000001E-4</v>
+      </c>
+      <c r="C26">
+        <v>-4.0474E-4</v>
+      </c>
+      <c r="D26">
+        <v>-2.2437999999999999E-4</v>
+      </c>
+      <c r="E26">
+        <v>8.8223299999999998E-3</v>
+      </c>
+      <c r="F26">
+        <v>3.150787E-2</v>
+      </c>
+      <c r="G26">
+        <v>8.7883000000000006E-3</v>
+      </c>
+      <c r="H26">
+        <v>1.0987149999999999E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17">
+      <c r="B27">
+        <v>8.7888900000000006E-3</v>
+      </c>
+      <c r="C27">
+        <v>-2.2440000000000001E-4</v>
+      </c>
+      <c r="D27">
+        <v>-3.6916E-4</v>
+      </c>
+      <c r="E27">
+        <v>-2.2437999999999999E-4</v>
+      </c>
+      <c r="F27">
+        <v>8.7883000000000006E-3</v>
+      </c>
+      <c r="G27">
+        <v>3.1591710000000002E-2</v>
+      </c>
+      <c r="H27">
+        <v>1.1084999999999999E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
+      <c r="B28">
+        <v>1.099497E-2</v>
+      </c>
+      <c r="C28">
+        <v>1.09871E-2</v>
+      </c>
+      <c r="D28">
+        <v>1.108454E-2</v>
+      </c>
+      <c r="E28">
+        <v>1.0995069999999999E-2</v>
+      </c>
+      <c r="F28">
+        <v>1.0987149999999999E-2</v>
+      </c>
+      <c r="G28">
+        <v>1.1084999999999999E-2</v>
+      </c>
+      <c r="H28">
+        <v>5.8237990000000003E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17">
+      <c r="A30" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17">
+      <c r="B31">
+        <v>2.1100899999999999E-2</v>
+      </c>
+      <c r="C31">
+        <v>-6.33257E-3</v>
+      </c>
+      <c r="D31">
+        <v>-6.3035399999999998E-3</v>
+      </c>
+      <c r="E31">
+        <v>-1.13671E-4</v>
+      </c>
+      <c r="F31">
+        <v>-1.13868E-4</v>
+      </c>
+      <c r="G31">
+        <v>-7.9919699999999993E-3</v>
+      </c>
+      <c r="H31">
+        <v>-2.4528000000000001E-4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17">
+      <c r="B32">
+        <v>-6.33257E-3</v>
+      </c>
+      <c r="C32">
+        <v>2.10926E-2</v>
+      </c>
+      <c r="D32">
+        <v>-1.13782E-4</v>
+      </c>
+      <c r="E32">
+        <v>-6.3041E-3</v>
+      </c>
+      <c r="F32">
+        <v>-2.44439E-4</v>
+      </c>
+      <c r="G32">
+        <v>-7.9838200000000008E-3</v>
+      </c>
+      <c r="H32">
+        <v>-1.13867E-4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="B33">
+        <v>-6.3035399999999998E-3</v>
+      </c>
+      <c r="C33">
+        <v>-1.13782E-4</v>
+      </c>
+      <c r="D33">
+        <v>2.11667E-2</v>
+      </c>
+      <c r="E33">
+        <v>-2.5288200000000001E-4</v>
+      </c>
+      <c r="F33">
+        <v>-6.30409E-3</v>
+      </c>
+      <c r="G33">
+        <v>-8.0787600000000008E-3</v>
+      </c>
+      <c r="H33">
+        <v>-1.13671E-4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="B34">
+        <v>-1.13671E-4</v>
+      </c>
+      <c r="C34">
+        <v>-6.3041E-3</v>
+      </c>
+      <c r="D34">
+        <v>-2.5288200000000001E-4</v>
+      </c>
+      <c r="E34">
+        <v>2.11662E-2</v>
+      </c>
+      <c r="F34">
+        <v>-1.1378E-4</v>
+      </c>
+      <c r="G34">
+        <v>-8.0782700000000002E-3</v>
+      </c>
+      <c r="H34">
+        <v>-6.30352E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="B35">
+        <v>-1.13868E-4</v>
+      </c>
+      <c r="C35">
+        <v>-2.44439E-4</v>
+      </c>
+      <c r="D35">
+        <v>-6.30409E-3</v>
+      </c>
+      <c r="E35">
+        <v>-1.1378E-4</v>
+      </c>
+      <c r="F35">
+        <v>2.10926E-2</v>
+      </c>
+      <c r="G35">
+        <v>-7.9838700000000005E-3</v>
+      </c>
+      <c r="H35">
+        <v>-6.33257E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="B36">
+        <v>-7.9919699999999993E-3</v>
+      </c>
+      <c r="C36">
+        <v>-7.9838200000000008E-3</v>
+      </c>
+      <c r="D36">
+        <v>-8.0787600000000008E-3</v>
+      </c>
+      <c r="E36">
+        <v>-8.0782700000000002E-3</v>
+      </c>
+      <c r="F36">
+        <v>-7.9838700000000005E-3</v>
+      </c>
+      <c r="G36">
+        <v>4.8108699999999997E-2</v>
+      </c>
+      <c r="H36">
+        <v>-7.9920100000000008E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="B37">
+        <v>-2.4528000000000001E-4</v>
+      </c>
+      <c r="C37">
+        <v>-1.13867E-4</v>
+      </c>
+      <c r="D37">
+        <v>-1.13671E-4</v>
+      </c>
+      <c r="E37">
+        <v>-6.30352E-3</v>
+      </c>
+      <c r="F37">
+        <v>-6.33257E-3</v>
+      </c>
+      <c r="G37">
+        <v>-7.9920100000000008E-3</v>
+      </c>
+      <c r="H37">
+        <v>2.1100899999999999E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" t="s">
+        <v>13</v>
+      </c>
+      <c r="B39" t="s">
+        <v>35</v>
+      </c>
+      <c r="C39" s="174">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D39" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="B40">
+        <v>3.0864260000000001E-2</v>
+      </c>
+      <c r="C40">
+        <v>9.1756700000000004E-3</v>
+      </c>
+      <c r="D40">
+        <v>9.1379900000000003E-3</v>
+      </c>
+      <c r="E40">
+        <v>-2.0937000000000001E-4</v>
+      </c>
+      <c r="F40">
+        <v>-2.1138E-4</v>
+      </c>
+      <c r="G40">
+        <v>1.1617300000000001E-2</v>
+      </c>
+      <c r="H40">
+        <v>-1.6823000000000001E-4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="B41">
+        <v>9.1756700000000004E-3</v>
+      </c>
+      <c r="C41">
+        <v>3.081745E-2</v>
+      </c>
+      <c r="D41">
+        <v>-2.1102999999999999E-4</v>
+      </c>
+      <c r="E41">
+        <v>9.1399199999999993E-3</v>
+      </c>
+      <c r="F41">
+        <v>-1.7273000000000001E-4</v>
+      </c>
+      <c r="G41">
+        <v>1.1574839999999999E-2</v>
+      </c>
+      <c r="H41">
+        <v>-2.1100000000000001E-4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="B42">
+        <v>9.1379900000000003E-3</v>
+      </c>
+      <c r="C42">
+        <v>-2.1102999999999999E-4</v>
+      </c>
+      <c r="D42">
+        <v>3.099828E-2</v>
+      </c>
+      <c r="E42">
+        <v>-1.5027000000000001E-4</v>
+      </c>
+      <c r="F42">
+        <v>9.1419399999999994E-3</v>
+      </c>
+      <c r="G42">
+        <v>1.1753629999999999E-2</v>
+      </c>
+      <c r="H42">
+        <v>-2.0901000000000001E-4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="B43">
+        <v>-2.0937000000000001E-4</v>
+      </c>
+      <c r="C43">
+        <v>9.1399199999999993E-3</v>
+      </c>
+      <c r="D43">
+        <v>-1.5027000000000001E-4</v>
+      </c>
+      <c r="E43">
+        <v>3.099207E-2</v>
+      </c>
+      <c r="F43">
+        <v>-2.1131000000000001E-4</v>
+      </c>
+      <c r="G43">
+        <v>1.175149E-2</v>
+      </c>
+      <c r="H43">
+        <v>9.1373400000000007E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="B44">
+        <v>-2.1138E-4</v>
+      </c>
+      <c r="C44">
+        <v>-1.7273000000000001E-4</v>
+      </c>
+      <c r="D44">
+        <v>9.1419399999999994E-3</v>
+      </c>
+      <c r="E44">
+        <v>-2.1131000000000001E-4</v>
+      </c>
+      <c r="F44">
+        <v>3.082064E-2</v>
+      </c>
+      <c r="G44">
+        <v>1.1578130000000001E-2</v>
+      </c>
+      <c r="H44">
+        <v>9.1741400000000008E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="B45">
+        <v>1.1617300000000001E-2</v>
+      </c>
+      <c r="C45">
+        <v>1.1574839999999999E-2</v>
+      </c>
+      <c r="D45">
+        <v>1.1753629999999999E-2</v>
+      </c>
+      <c r="E45">
+        <v>1.175149E-2</v>
+      </c>
+      <c r="F45">
+        <v>1.1578130000000001E-2</v>
+      </c>
+      <c r="G45">
+        <v>7.1350780000000003E-2</v>
+      </c>
+      <c r="H45">
+        <v>1.1617840000000001E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="B46">
+        <v>-1.6823000000000001E-4</v>
+      </c>
+      <c r="C46">
+        <v>-2.1100000000000001E-4</v>
+      </c>
+      <c r="D46">
+        <v>-2.0901000000000001E-4</v>
+      </c>
+      <c r="E46">
+        <v>9.1373400000000007E-3</v>
+      </c>
+      <c r="F46">
+        <v>9.1741400000000008E-3</v>
+      </c>
+      <c r="G46">
+        <v>1.1617840000000001E-2</v>
+      </c>
+      <c r="H46">
+        <v>3.086289E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>